<commit_message>
치트 GMLEVEL 체크 수정 hero_bg.png삭제
</commit_message>
<xml_diff>
--- a/패치플로우.xlsx
+++ b/패치플로우.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>리소스패치</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -191,6 +191,58 @@
   </si>
   <si>
     <t>클라이언트로 패치 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버앱 패치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>젠킨스 실행(193번서버의…)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 소스 GIT-master에 commit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빌드시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료되면 실행파일이 GMO서버의 share폴더로 간다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GMO서버 접속</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desktop/share폴더 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버앱패치.bat 실행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백업은 자동으로 이뤄진다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버리소스 패치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resouce/서버패치용_카피.bat 실행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버앱에 필요한 리소스를 GMO/share폴더에 업로드 한다.(리눅스 경유)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버리소스패치.bat 실행</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -198,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +284,15 @@
     </font>
     <font>
       <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -291,7 +352,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -307,9 +368,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -320,6 +387,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -626,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -1073,89 +1149,206 @@
       <c r="P22" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="6">
+    <row r="40" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
         <v>1</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G40" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="5">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
         <v>2</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="8">
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10">
         <v>3</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="8">
+      <c r="G42" s="13"/>
+    </row>
+    <row r="43" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10">
         <v>4</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="9">
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="11">
         <v>5</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G44" s="9" t="s">
+      <c r="G44" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5">
+    <row r="45" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
         <v>6</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="8">
+      <c r="G45" s="7"/>
+    </row>
+    <row r="46" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10">
         <v>7</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="8">
+      <c r="G46" s="13"/>
+    </row>
+    <row r="47" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="10">
         <v>8</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G47" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="9">
+    <row r="48" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="11">
         <v>9</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="11" t="s">
         <v>42</v>
+      </c>
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6">
+        <v>1</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G51" s="7"/>
+    </row>
+    <row r="52" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10">
+        <v>2</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G52" s="13"/>
+    </row>
+    <row r="53" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="11">
+        <v>3</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G53" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6">
+        <v>4</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="10">
+        <v>5</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G55" s="13"/>
+    </row>
+    <row r="56" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="11">
+        <v>6</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="8">
+        <v>1</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="6">
+        <v>2</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="10">
+        <v>3</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="11">
+        <v>4</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>